<commit_message>
added datasets, graphs, conclusions, and commented requests
</commit_message>
<xml_diff>
--- a/predictive_data/snack_data.xlsx
+++ b/predictive_data/snack_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17400" yWindow="460" windowWidth="11660" windowHeight="16420" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="18800" yWindow="460" windowWidth="10000" windowHeight="16340" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
   <si>
     <t>Potato Chips</t>
   </si>
@@ -804,7 +804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -858,10 +860,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,22 +872,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="3">
-        <v>45.4</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3">
-        <v>32.200000000000003</v>
+        <v>45.4</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -893,10 +892,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3">
-        <v>31.5</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -904,10 +903,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
-        <v>25</v>
+        <v>31.5</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -915,10 +914,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3">
-        <v>24.3</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -926,10 +925,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3">
-        <v>24.1</v>
+        <v>24.3</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -937,32 +936,32 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3">
-        <v>22.4</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>24.1</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3">
-        <v>19.2</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>22.4</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3">
-        <v>17.399999999999999</v>
+        <v>19.2</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -970,10 +969,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="3">
-        <v>16.5</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -981,66 +980,66 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="C11" s="4"/>
+        <v>16.5</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3">
-        <v>31.3</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3">
-        <v>28.1</v>
+        <v>31.3</v>
       </c>
       <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="3">
-        <v>25.2</v>
+        <v>28.1</v>
       </c>
       <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="3">
-        <v>24</v>
+        <v>25.2</v>
       </c>
       <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="3">
-        <v>11.5</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="3">
-        <v>11.4</v>
+        <v>11.5</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1048,10 +1047,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="3">
-        <v>10.9</v>
+        <v>11.4</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1059,10 +1058,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="3">
-        <v>9.1</v>
+        <v>10.9</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1070,10 +1069,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3">
-        <v>8.6</v>
+        <v>9.1</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1081,10 +1080,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" s="3">
-        <v>25</v>
+        <v>8.6</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1092,10 +1091,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="3">
-        <v>14.1</v>
+        <v>25</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1103,21 +1102,29 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B24" s="3">
         <v>11.8</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="2">
-        <f>SUM(B1:B23)</f>
-        <v>501.30000000000007</v>
-      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1126,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" activeCellId="1" sqref="B22 A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1138,22 +1145,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="3">
-        <v>52.3</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="4"/>
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3">
-        <v>40.700000000000003</v>
+        <v>52.3</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1"/>
@@ -1161,10 +1165,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3">
-        <v>37.299999999999997</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
@@ -1172,10 +1176,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3">
-        <v>30.3</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
@@ -1183,10 +1187,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3">
-        <v>29.2</v>
+        <v>30.3</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="1"/>
@@ -1194,10 +1198,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3">
-        <v>22.9</v>
+        <v>29.2</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="1"/>
@@ -1205,10 +1209,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3">
-        <v>19.600000000000001</v>
+        <v>22.9</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="1"/>
@@ -1216,10 +1220,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="3">
-        <v>18</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="1"/>
@@ -1227,10 +1231,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3">
-        <v>16.399999999999999</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1"/>
@@ -1238,10 +1242,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3">
-        <v>14.2</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="1"/>
@@ -1249,32 +1253,32 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="3">
-        <v>38</v>
+        <v>14.2</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="3">
-        <v>30.1</v>
+        <v>38</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3">
-        <v>25.7</v>
+        <v>30.1</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="1"/>
@@ -1282,10 +1286,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3">
-        <v>20.8</v>
+        <v>25.7</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1"/>
@@ -1293,10 +1297,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="3">
-        <v>20</v>
+        <v>20.8</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
@@ -1304,10 +1308,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3">
-        <v>40.799999999999997</v>
+        <v>20</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1"/>
@@ -1315,10 +1319,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3">
-        <v>29.1</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1"/>
@@ -1326,10 +1330,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="3">
-        <v>27.6</v>
+        <v>29.1</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="1"/>
@@ -1337,10 +1341,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="3">
-        <v>25.2</v>
+        <v>27.6</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1"/>
@@ -1348,20 +1352,28 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="3">
-        <v>21.4</v>
+        <v>25.2</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="1"/>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="2">
-        <f>SUM(B1:B20)</f>
-        <v>559.6</v>
-      </c>
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="3">
+        <v>21.4</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1370,7 +1382,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
@@ -1382,22 +1394,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="3">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="4"/>
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="3">
-        <v>14.2</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1"/>
@@ -1405,54 +1414,54 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="3">
-        <v>12.1</v>
-      </c>
-      <c r="C3" s="1"/>
+        <v>14.2</v>
+      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3">
-        <v>11.9</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>12.1</v>
+      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3">
-        <v>11.2</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>11.9</v>
+      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>11.2</v>
+      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="3">
-        <v>7.4</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="1"/>
@@ -1460,32 +1469,32 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="3">
-        <v>6.6</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>7.4</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="C9" s="4"/>
+        <v>6.6</v>
+      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="3">
-        <v>5.7</v>
+        <v>6.1</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="1"/>
@@ -1493,10 +1502,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="3">
-        <v>5.5</v>
+        <v>5.7</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1"/>
@@ -1504,10 +1513,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="3">
-        <v>21.3</v>
+        <v>5.5</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1"/>
@@ -1515,10 +1524,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="3">
-        <v>17.600000000000001</v>
+        <v>21.3</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="1"/>
@@ -1526,10 +1535,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" s="3">
-        <v>28.1</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1"/>
@@ -1537,10 +1546,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B15" s="3">
-        <v>24.7</v>
+        <v>28.1</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
@@ -1548,21 +1557,29 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B16" s="3">
-        <v>23.4</v>
+        <v>24.7</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="2">
-        <f>SUM(B1:B16)</f>
-        <v>222.89999999999998</v>
-      </c>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="3">
+        <v>23.4</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1571,7 +1588,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -1583,22 +1600,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="3">
-        <v>24.3</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="4"/>
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3">
-        <v>24.2</v>
+        <v>24.3</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1"/>
@@ -1606,10 +1620,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3">
-        <v>22</v>
+        <v>24.2</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="1"/>
@@ -1617,10 +1631,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3">
-        <v>20.5</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="1"/>
@@ -1628,10 +1642,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="3">
-        <v>19.5</v>
+        <v>20.5</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="1"/>
@@ -1639,32 +1653,32 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3">
-        <v>15.8</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>19.5</v>
+      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="3">
-        <v>15.6</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>15.8</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="3">
-        <v>14.2</v>
+        <v>15.6</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="1"/>
@@ -1672,10 +1686,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="3">
-        <v>13.4</v>
+        <v>14.2</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="1"/>
@@ -1683,10 +1697,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="3">
-        <v>12.5</v>
+        <v>13.4</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="1"/>
@@ -1694,10 +1708,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="3">
-        <v>70.7</v>
+        <v>12.5</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="1"/>
@@ -1705,10 +1719,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="3">
-        <v>29.7</v>
+        <v>70.7</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="1"/>
@@ -1716,10 +1730,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="3">
-        <v>10.1</v>
+        <v>29.7</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="1"/>
@@ -1727,10 +1741,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="3">
-        <v>9.1</v>
+        <v>10.1</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="1"/>
@@ -1738,10 +1752,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="3">
-        <v>8.1999999999999993</v>
+        <v>9.1</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
@@ -1749,10 +1763,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B16" s="3">
-        <v>19.5</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="1"/>
@@ -1760,10 +1774,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" s="3">
-        <v>15.6</v>
+        <v>19.5</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="1"/>
@@ -1771,10 +1785,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="3">
-        <v>14.2</v>
+        <v>15.6</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="1"/>
@@ -1782,10 +1796,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" s="3">
-        <v>12.5</v>
+        <v>14.2</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="1"/>
@@ -1793,21 +1807,29 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B20" s="3">
-        <v>11.9</v>
+        <v>12.5</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-      <c r="B21" s="2">
-        <f>SUM(B1:B20)</f>
-        <v>383.5</v>
-      </c>
+      <c r="A21" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added data science files
</commit_message>
<xml_diff>
--- a/predictive_data/snack_data.xlsx
+++ b/predictive_data/snack_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="460" windowWidth="10000" windowHeight="16340" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="18800" yWindow="460" windowWidth="10000" windowHeight="16300" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="169">
   <si>
     <t>Potato Chips</t>
   </si>
@@ -320,6 +320,225 @@
   </si>
   <si>
     <t>Snack</t>
+  </si>
+  <si>
+    <t>B018QU0E38</t>
+  </si>
+  <si>
+    <t>B01N0SS46Z</t>
+  </si>
+  <si>
+    <t>B000UESJ8Q</t>
+  </si>
+  <si>
+    <t>B014JSQ228</t>
+  </si>
+  <si>
+    <t>B01MY05VGS</t>
+  </si>
+  <si>
+    <t>B008ZX8STY</t>
+  </si>
+  <si>
+    <t>B014JSQ4RG</t>
+  </si>
+  <si>
+    <t>B017ALD6SY</t>
+  </si>
+  <si>
+    <t>B012UO5GXE</t>
+  </si>
+  <si>
+    <t>B00MUFHJMK</t>
+  </si>
+  <si>
+    <t>B00W0C9F5M</t>
+  </si>
+  <si>
+    <t>B00J50Q212</t>
+  </si>
+  <si>
+    <t>B004SKOOXC</t>
+  </si>
+  <si>
+    <t>B00I8QZN1O</t>
+  </si>
+  <si>
+    <t>B01N7T2S72</t>
+  </si>
+  <si>
+    <t>B01NBVMFEQ</t>
+  </si>
+  <si>
+    <t>B00TS9LWK6</t>
+  </si>
+  <si>
+    <t>B019KE3616</t>
+  </si>
+  <si>
+    <t>B019KFB1OY</t>
+  </si>
+  <si>
+    <t>B01N5Q8Y6H</t>
+  </si>
+  <si>
+    <t>B01N23A83E</t>
+  </si>
+  <si>
+    <t>B00VDIRR2C</t>
+  </si>
+  <si>
+    <t>B00AHHEEKI</t>
+  </si>
+  <si>
+    <t>B00AHHEECQ</t>
+  </si>
+  <si>
+    <t>B00AHHEEDA</t>
+  </si>
+  <si>
+    <t>B00C8T50GU</t>
+  </si>
+  <si>
+    <t>B00MHYJZ3A</t>
+  </si>
+  <si>
+    <t>B00LPDFME0</t>
+  </si>
+  <si>
+    <t>B00M63DP0G</t>
+  </si>
+  <si>
+    <t>B00OVDQN4E</t>
+  </si>
+  <si>
+    <t>B001C5XE1O</t>
+  </si>
+  <si>
+    <t>B01HBZXNPK</t>
+  </si>
+  <si>
+    <t>B01JCW3314</t>
+  </si>
+  <si>
+    <t>B00AH7LMBM</t>
+  </si>
+  <si>
+    <t>B00VOF8O0I</t>
+  </si>
+  <si>
+    <t>B00QJGU798</t>
+  </si>
+  <si>
+    <t>B071XC8DSW</t>
+  </si>
+  <si>
+    <t>B00QAL5CPQ</t>
+  </si>
+  <si>
+    <t>B00PB0JC5I</t>
+  </si>
+  <si>
+    <t>B00QJGVF4Y</t>
+  </si>
+  <si>
+    <t>B00QJGV64I</t>
+  </si>
+  <si>
+    <t>B001TKF3NY</t>
+  </si>
+  <si>
+    <t>B00HDC09OA</t>
+  </si>
+  <si>
+    <t>B000RI1W8E</t>
+  </si>
+  <si>
+    <t>B00WDWXHQ2</t>
+  </si>
+  <si>
+    <t>B01M8ME082</t>
+  </si>
+  <si>
+    <t>B000GW0U3E</t>
+  </si>
+  <si>
+    <t>B000GW6786</t>
+  </si>
+  <si>
+    <t>B01CT6FKKW</t>
+  </si>
+  <si>
+    <t>B000CQID1K</t>
+  </si>
+  <si>
+    <t>B00VB1X1HG</t>
+  </si>
+  <si>
+    <t>B00NLHBPHG</t>
+  </si>
+  <si>
+    <t>B001IZEJ76</t>
+  </si>
+  <si>
+    <t>B01CT6FLAQ</t>
+  </si>
+  <si>
+    <t>B002OFU7MK</t>
+  </si>
+  <si>
+    <t>B00WR27RDM</t>
+  </si>
+  <si>
+    <t>B002RTW5B4</t>
+  </si>
+  <si>
+    <t>B0054RPY7I</t>
+  </si>
+  <si>
+    <t>B001QCUKII</t>
+  </si>
+  <si>
+    <t>B001G7RDRO</t>
+  </si>
+  <si>
+    <t>B001E7654S</t>
+  </si>
+  <si>
+    <t>B00I0DI0Z6</t>
+  </si>
+  <si>
+    <t>B009VV7G60</t>
+  </si>
+  <si>
+    <t>B00WOBPLIE</t>
+  </si>
+  <si>
+    <t>B002YM58UE</t>
+  </si>
+  <si>
+    <t>B003TNANSO</t>
+  </si>
+  <si>
+    <t>B00VQI9ITE</t>
+  </si>
+  <si>
+    <t>B000YW7Q0Q</t>
+  </si>
+  <si>
+    <t>B00BSW6LH0</t>
+  </si>
+  <si>
+    <t>B00BQ15C1O</t>
+  </si>
+  <si>
+    <t>B00469S5YY</t>
+  </si>
+  <si>
+    <t>B004M4W80U</t>
+  </si>
+  <si>
+    <t>B009VV7A9I</t>
   </si>
 </sst>
 </file>
@@ -329,7 +548,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -357,6 +576,22 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -375,8 +610,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -388,7 +627,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -862,13 +1105,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -886,7 +1130,9 @@
       <c r="B2" s="3">
         <v>45.4</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
@@ -897,7 +1143,9 @@
       <c r="B3" s="3">
         <v>32.200000000000003</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
@@ -908,7 +1156,9 @@
       <c r="B4" s="3">
         <v>31.5</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
@@ -919,7 +1169,9 @@
       <c r="B5" s="3">
         <v>25</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
@@ -930,7 +1182,9 @@
       <c r="B6" s="3">
         <v>24.3</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
@@ -941,7 +1195,9 @@
       <c r="B7" s="3">
         <v>24.1</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
@@ -952,7 +1208,9 @@
       <c r="B8" s="3">
         <v>22.4</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
@@ -963,7 +1221,9 @@
       <c r="B9" s="3">
         <v>19.2</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
@@ -974,7 +1234,9 @@
       <c r="B10" s="3">
         <v>17.399999999999999</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
@@ -985,7 +1247,9 @@
       <c r="B11" s="3">
         <v>16.5</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
@@ -996,7 +1260,9 @@
       <c r="B12" s="3">
         <v>32.299999999999997</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -1005,7 +1271,9 @@
       <c r="B13" s="3">
         <v>31.3</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -1014,7 +1282,9 @@
       <c r="B14" s="3">
         <v>28.1</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -1023,7 +1293,9 @@
       <c r="B15" s="3">
         <v>25.2</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1032,7 +1304,9 @@
       <c r="B16" s="3">
         <v>24</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -1041,7 +1315,9 @@
       <c r="B17" s="3">
         <v>11.5</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>110</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
@@ -1052,7 +1328,9 @@
       <c r="B18" s="3">
         <v>11.4</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
@@ -1063,7 +1341,9 @@
       <c r="B19" s="3">
         <v>10.9</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
@@ -1074,7 +1354,9 @@
       <c r="B20" s="3">
         <v>9.1</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
@@ -1085,7 +1367,9 @@
       <c r="B21" s="3">
         <v>8.6</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
@@ -1096,7 +1380,9 @@
       <c r="B22" s="3">
         <v>25</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>115</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
@@ -1107,7 +1393,9 @@
       <c r="B23" s="3">
         <v>14.1</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
@@ -1118,7 +1406,9 @@
       <c r="B24" s="3">
         <v>11.8</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="4"/>
     </row>
@@ -1128,6 +1418,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1135,13 +1426,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" activeCellId="1" sqref="B22 A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.5" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1159,7 +1451,9 @@
       <c r="B2" s="3">
         <v>52.3</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="4"/>
     </row>
@@ -1170,7 +1464,9 @@
       <c r="B3" s="3">
         <v>40.700000000000003</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="4"/>
     </row>
@@ -1181,7 +1477,9 @@
       <c r="B4" s="3">
         <v>37.299999999999997</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
     </row>
@@ -1192,7 +1490,9 @@
       <c r="B5" s="3">
         <v>30.3</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
@@ -1203,7 +1503,9 @@
       <c r="B6" s="3">
         <v>29.2</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
@@ -1214,7 +1516,9 @@
       <c r="B7" s="3">
         <v>22.9</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
@@ -1225,7 +1529,9 @@
       <c r="B8" s="3">
         <v>19.600000000000001</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
@@ -1236,7 +1542,9 @@
       <c r="B9" s="3">
         <v>18</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
     </row>
@@ -1247,7 +1555,9 @@
       <c r="B10" s="3">
         <v>16.399999999999999</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
@@ -1258,7 +1568,9 @@
       <c r="B11" s="3">
         <v>14.2</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
@@ -1269,7 +1581,9 @@
       <c r="B12" s="3">
         <v>38</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="7"/>
     </row>
@@ -1280,7 +1594,9 @@
       <c r="B13" s="3">
         <v>30.1</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
@@ -1291,7 +1607,9 @@
       <c r="B14" s="3">
         <v>25.7</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="4"/>
     </row>
@@ -1302,7 +1620,9 @@
       <c r="B15" s="3">
         <v>20.8</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="4"/>
     </row>
@@ -1313,7 +1633,9 @@
       <c r="B16" s="3">
         <v>20</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="4"/>
     </row>
@@ -1324,7 +1646,9 @@
       <c r="B17" s="3">
         <v>40.799999999999997</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="4"/>
     </row>
@@ -1335,7 +1659,9 @@
       <c r="B18" s="3">
         <v>29.1</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="4"/>
     </row>
@@ -1346,7 +1672,9 @@
       <c r="B19" s="3">
         <v>27.6</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="4"/>
     </row>
@@ -1357,7 +1685,9 @@
       <c r="B20" s="3">
         <v>25.2</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="4"/>
     </row>
@@ -1368,7 +1698,9 @@
       <c r="B21" s="3">
         <v>21.4</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>137</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="4"/>
     </row>
@@ -1385,12 +1717,13 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1408,7 +1741,9 @@
       <c r="B2" s="3">
         <v>17.100000000000001</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="4"/>
     </row>
@@ -1419,7 +1754,9 @@
       <c r="B3" s="3">
         <v>14.2</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="4"/>
     </row>
@@ -1430,7 +1767,9 @@
       <c r="B4" s="3">
         <v>12.1</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
@@ -1441,7 +1780,9 @@
       <c r="B5" s="3">
         <v>11.9</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>141</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
@@ -1452,7 +1793,9 @@
       <c r="B6" s="3">
         <v>11.2</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>146</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
@@ -1463,7 +1806,9 @@
       <c r="B7" s="3">
         <v>10</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
@@ -1474,7 +1819,9 @@
       <c r="B8" s="3">
         <v>7.4</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
@@ -1485,7 +1832,9 @@
       <c r="B9" s="3">
         <v>6.6</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
@@ -1496,7 +1845,9 @@
       <c r="B10" s="3">
         <v>6.1</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
@@ -1507,7 +1858,9 @@
       <c r="B11" s="3">
         <v>5.7</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>147</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
@@ -1518,7 +1871,9 @@
       <c r="B12" s="3">
         <v>5.5</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
     </row>
@@ -1529,7 +1884,9 @@
       <c r="B13" s="3">
         <v>21.3</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
@@ -1540,7 +1897,9 @@
       <c r="B14" s="3">
         <v>17.600000000000001</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="4"/>
     </row>
@@ -1551,7 +1910,9 @@
       <c r="B15" s="3">
         <v>28.1</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="4"/>
     </row>
@@ -1562,7 +1923,9 @@
       <c r="B16" s="3">
         <v>24.7</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>145</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="4"/>
     </row>
@@ -1573,7 +1936,9 @@
       <c r="B17" s="3">
         <v>23.4</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>152</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="4"/>
     </row>
@@ -1591,12 +1956,13 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.5" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1614,7 +1980,9 @@
       <c r="B2" s="3">
         <v>24.3</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="4"/>
     </row>
@@ -1625,7 +1993,9 @@
       <c r="B3" s="3">
         <v>24.2</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="4"/>
     </row>
@@ -1636,7 +2006,9 @@
       <c r="B4" s="3">
         <v>22</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>155</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="4"/>
     </row>
@@ -1647,7 +2019,9 @@
       <c r="B5" s="3">
         <v>20.5</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>156</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="4"/>
     </row>
@@ -1658,7 +2032,9 @@
       <c r="B6" s="3">
         <v>19.5</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="4"/>
     </row>
@@ -1669,7 +2045,9 @@
       <c r="B7" s="3">
         <v>15.8</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="4"/>
     </row>
@@ -1680,7 +2058,9 @@
       <c r="B8" s="3">
         <v>15.6</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>158</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="4"/>
     </row>
@@ -1691,7 +2071,9 @@
       <c r="B9" s="3">
         <v>14.2</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>159</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="4"/>
     </row>
@@ -1702,7 +2084,9 @@
       <c r="B10" s="3">
         <v>13.4</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>161</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="4"/>
     </row>
@@ -1713,7 +2097,9 @@
       <c r="B11" s="3">
         <v>12.5</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="4"/>
     </row>
@@ -1724,7 +2110,9 @@
       <c r="B12" s="3">
         <v>70.7</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>163</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="4"/>
     </row>
@@ -1735,7 +2123,9 @@
       <c r="B13" s="3">
         <v>29.7</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>164</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="4"/>
     </row>
@@ -1746,7 +2136,9 @@
       <c r="B14" s="3">
         <v>10.1</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>165</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="4"/>
     </row>
@@ -1757,7 +2149,9 @@
       <c r="B15" s="3">
         <v>9.1</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="4"/>
     </row>
@@ -1768,7 +2162,9 @@
       <c r="B16" s="3">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="4"/>
     </row>
@@ -1779,7 +2175,9 @@
       <c r="B17" s="3">
         <v>19.5</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17" s="4"/>
     </row>
@@ -1790,7 +2188,9 @@
       <c r="B18" s="3">
         <v>15.6</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>158</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="4"/>
     </row>
@@ -1801,7 +2201,9 @@
       <c r="B19" s="3">
         <v>14.2</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>159</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="4"/>
     </row>
@@ -1812,7 +2214,9 @@
       <c r="B20" s="3">
         <v>12.5</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="4"/>
     </row>
@@ -1823,7 +2227,9 @@
       <c r="B21" s="3">
         <v>11.9</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>168</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>

</xml_diff>